<commit_message>
added one more user
</commit_message>
<xml_diff>
--- a/Python ETL/usuario_mock.xlsx
+++ b/Python ETL/usuario_mock.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/carolineamarante/Documents/gerenciamento-de-salas-V0.1/Python ETL/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A009FDA-DBD0-614C-8415-5218C821A383}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0FE613A-A7F1-0943-AC52-89385C1638FE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="80" yWindow="460" windowWidth="25440" windowHeight="14920" xr2:uid="{34CB7556-4D6D-0B47-B63C-C260E26F6C7A}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="11">
   <si>
     <t>email</t>
   </si>
@@ -58,6 +58,12 @@
   </si>
   <si>
     <t>admin@fatec.com</t>
+  </si>
+  <si>
+    <t>isaac@gmail.com</t>
+  </si>
+  <si>
+    <t>Password123$</t>
   </si>
 </sst>
 </file>
@@ -420,7 +426,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D17C5CB2-9692-4A4A-AE42-AFBCC0712D3F}">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
@@ -488,6 +494,14 @@
         <v>3</v>
       </c>
     </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" t="s">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" xr:uid="{47829436-A4F6-0446-82CA-6E84DEF7306E}"/>
@@ -501,6 +515,7 @@
     <hyperlink ref="A5" r:id="rId9" xr:uid="{CCEDC5FB-7682-244B-BF39-32B5D33AF1BB}"/>
     <hyperlink ref="A6" r:id="rId10" xr:uid="{3F8CF56B-B76A-FF4C-BBC3-AB7E1C8B7B64}"/>
     <hyperlink ref="B7" r:id="rId11" xr:uid="{11DFCFE0-AA02-5F40-B1BD-0C8322C3097D}"/>
+    <hyperlink ref="A8" r:id="rId12" xr:uid="{2F789AA3-E544-BB42-91A7-AD3E27312683}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
fixed many thiong son register screen and styles for alunos
</commit_message>
<xml_diff>
--- a/Python ETL/usuario_mock.xlsx
+++ b/Python ETL/usuario_mock.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10908"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/carolineamarante/Documents/gerenciamento-de-salas-V0.1/Python ETL/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Isaac\Documents\GitHub\gerenciamento-de-salas-V0.1\Python ETL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7EB9AC9-6096-EB40-9EE9-5D54FCCAD77D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFC9F0FE-FBFC-4EF5-929C-A510EB56B4AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="460" windowWidth="18200" windowHeight="8500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1560" yWindow="1560" windowWidth="21600" windowHeight="11505" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -65,7 +65,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -75,18 +75,23 @@
     </font>
     <font>
       <u/>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <u/>
       <sz val="11"/>
       <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aharoni"/>
+      <charset val="177"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Aharoni"/>
+      <charset val="177"/>
     </font>
   </fonts>
   <fills count="2">
@@ -115,31 +120,102 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="5">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Aharoni"/>
+        <charset val="177"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <vertAlign val="baseline"/>
+        <name val="Aharoni"/>
+        <charset val="177"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <color theme="1"/>
+        <name val="Aharoni"/>
+        <charset val="177"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <vertAlign val="baseline"/>
+        <name val="Aharoni"/>
+        <charset val="177"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <vertAlign val="baseline"/>
+        <name val="Aharoni"/>
+        <charset val="177"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -150,6 +226,18 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{82784D4B-A787-48F4-8B9F-3232D5FE215D}" name="Tabela1" displayName="Tabela1" ref="A1:C6" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3">
+  <autoFilter ref="A1:C6" xr:uid="{82784D4B-A787-48F4-8B9F-3232D5FE215D}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{08F46135-D8DD-440A-9E7B-D2A7B9CD0D09}" name="email" dataDxfId="2" dataCellStyle="Hiperlink"/>
+    <tableColumn id="2" xr3:uid="{123EA1D0-7E32-45F8-8D58-AA814E57942B}" name="senha" dataDxfId="0"/>
+    <tableColumn id="3" xr3:uid="{E5A03E2E-8A94-4513-8E51-83D6F010941E}" name="role" dataDxfId="1"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -443,78 +531,79 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.1640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="32" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.7109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="17.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:3" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
+    <row r="3" spans="1:3" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="2" t="s">
         <v>12</v>
       </c>
     </row>
@@ -525,5 +614,8 @@
     <hyperlink ref="A6" r:id="rId3" xr:uid="{5ED3BFB0-8F91-394B-A682-48673A8ADAF4}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId4"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>